<commit_message>
commiting log4j to branchx
</commit_message>
<xml_diff>
--- a/src/test/Files/excel/testdata.xlsx
+++ b/src/test/Files/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" state="visible" r:id="rId2"/>
@@ -503,8 +503,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="105" zoomScaleNormal="105" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,8 +628,8 @@
   </sheetPr>
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>